<commit_message>
Nivel de usuarios e Informacion del equipo realizado
Nivel de usuarios e Informacion del equipo realizado
</commit_message>
<xml_diff>
--- a/Documentos/Tabla de Agencias.xlsx
+++ b/Documentos/Tabla de Agencias.xlsx
@@ -6,13 +6,13 @@
     <x:workbookView/>
   </x:bookViews>
   <x:sheets>
-    <x:sheet name="Sheet1" sheetId="1" r:id="Rd9b8c1700adc4613"/>
+    <x:sheet name="Sheet1" sheetId="1" r:id="R1cdf9914a34d47a4"/>
   </x:sheets>
 </x:workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
   <x:si>
     <x:t>#</x:t>
   </x:si>
@@ -35,7 +35,7 @@
     <x:t>EA Sports</x:t>
   </x:si>
   <x:si>
-    <x:t>Deportivo</x:t>
+    <x:t>Deportiva</x:t>
   </x:si>
   <x:si>
     <x:t>555-1234</x:t>
@@ -44,6 +44,72 @@
     <x:t>contacto@easports.com</x:t>
   </x:si>
   <x:si>
+    <x:t>6</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Bwin</x:t>
+  </x:si>
+  <x:si>
+    <x:t>555-3456</x:t>
+  </x:si>
+  <x:si>
+    <x:t>support@bwin.com</x:t>
+  </x:si>
+  <x:si>
+    <x:t>5</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Adidas</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Publicidad</x:t>
+  </x:si>
+  <x:si>
+    <x:t>555-2345</x:t>
+  </x:si>
+  <x:si>
+    <x:t>service@adidas.com</x:t>
+  </x:si>
+  <x:si>
+    <x:t>8</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Puma</x:t>
+  </x:si>
+  <x:si>
+    <x:t>555-7890</x:t>
+  </x:si>
+  <x:si>
+    <x:t>contact@puma.com</x:t>
+  </x:si>
+  <x:si>
+    <x:t>3</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Nike</x:t>
+  </x:si>
+  <x:si>
+    <x:t>555-8765</x:t>
+  </x:si>
+  <x:si>
+    <x:t>support@nike.com</x:t>
+  </x:si>
+  <x:si>
+    <x:t>4</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Fox Sports</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Televisión</x:t>
+  </x:si>
+  <x:si>
+    <x:t>555-4321</x:t>
+  </x:si>
+  <x:si>
+    <x:t>info@foxsports.com</x:t>
+  </x:si>
+  <x:si>
     <x:t>2</x:t>
   </x:si>
   <x:si>
@@ -56,54 +122,6 @@
     <x:t>info@espn.com</x:t>
   </x:si>
   <x:si>
-    <x:t>3</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Nike</x:t>
-  </x:si>
-  <x:si>
-    <x:t>555-8765</x:t>
-  </x:si>
-  <x:si>
-    <x:t>support@nike.com</x:t>
-  </x:si>
-  <x:si>
-    <x:t>4</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Fox Sports</x:t>
-  </x:si>
-  <x:si>
-    <x:t>555-4321</x:t>
-  </x:si>
-  <x:si>
-    <x:t>info@foxsports.com</x:t>
-  </x:si>
-  <x:si>
-    <x:t>5</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Adidas</x:t>
-  </x:si>
-  <x:si>
-    <x:t>555-2345</x:t>
-  </x:si>
-  <x:si>
-    <x:t>service@adidas.com</x:t>
-  </x:si>
-  <x:si>
-    <x:t>6</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Bwin</x:t>
-  </x:si>
-  <x:si>
-    <x:t>555-3456</x:t>
-  </x:si>
-  <x:si>
-    <x:t>support@bwin.com</x:t>
-  </x:si>
-  <x:si>
     <x:t>7</x:t>
   </x:si>
   <x:si>
@@ -114,18 +132,6 @@
   </x:si>
   <x:si>
     <x:t>info@telemundo.com</x:t>
-  </x:si>
-  <x:si>
-    <x:t>8</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Puma</x:t>
-  </x:si>
-  <x:si>
-    <x:t>555-7890</x:t>
-  </x:si>
-  <x:si>
-    <x:t>contact@puma.com</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -490,7 +496,7 @@
   <x:cols>
     <x:col min="1" max="1" width="2.28515625" bestFit="1" customWidth="1"/>
     <x:col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
-    <x:col min="3" max="3" width="9.85546875" bestFit="1" customWidth="1"/>
+    <x:col min="3" max="3" width="10.140625" bestFit="1" customWidth="1"/>
     <x:col min="4" max="4" width="9.7109375" bestFit="1" customWidth="1"/>
     <x:col min="5" max="5" width="22.5703125" bestFit="1" customWidth="1"/>
   </x:cols>
@@ -554,98 +560,98 @@
         <x:v>15</x:v>
       </x:c>
       <x:c r="C4" s="4" t="s">
-        <x:v>7</x:v>
+        <x:v>16</x:v>
       </x:c>
       <x:c r="D4" s="4" t="s">
-        <x:v>16</x:v>
+        <x:v>17</x:v>
       </x:c>
       <x:c r="E4" s="4" t="s">
-        <x:v>17</x:v>
+        <x:v>18</x:v>
       </x:c>
     </x:row>
     <x:row r="5">
       <x:c r="A5" s="4" t="s">
-        <x:v>18</x:v>
+        <x:v>19</x:v>
       </x:c>
       <x:c r="B5" s="4" t="s">
-        <x:v>19</x:v>
+        <x:v>20</x:v>
       </x:c>
       <x:c r="C5" s="4" t="s">
-        <x:v>7</x:v>
+        <x:v>16</x:v>
       </x:c>
       <x:c r="D5" s="4" t="s">
-        <x:v>20</x:v>
+        <x:v>21</x:v>
       </x:c>
       <x:c r="E5" s="4" t="s">
-        <x:v>21</x:v>
+        <x:v>22</x:v>
       </x:c>
     </x:row>
     <x:row r="6">
       <x:c r="A6" s="4" t="s">
-        <x:v>22</x:v>
+        <x:v>23</x:v>
       </x:c>
       <x:c r="B6" s="4" t="s">
-        <x:v>23</x:v>
+        <x:v>24</x:v>
       </x:c>
       <x:c r="C6" s="4" t="s">
-        <x:v>7</x:v>
+        <x:v>16</x:v>
       </x:c>
       <x:c r="D6" s="4" t="s">
-        <x:v>24</x:v>
+        <x:v>25</x:v>
       </x:c>
       <x:c r="E6" s="4" t="s">
-        <x:v>25</x:v>
+        <x:v>26</x:v>
       </x:c>
     </x:row>
     <x:row r="7">
       <x:c r="A7" s="4" t="s">
-        <x:v>26</x:v>
+        <x:v>27</x:v>
       </x:c>
       <x:c r="B7" s="4" t="s">
-        <x:v>27</x:v>
+        <x:v>28</x:v>
       </x:c>
       <x:c r="C7" s="4" t="s">
-        <x:v>7</x:v>
+        <x:v>29</x:v>
       </x:c>
       <x:c r="D7" s="4" t="s">
-        <x:v>28</x:v>
+        <x:v>30</x:v>
       </x:c>
       <x:c r="E7" s="4" t="s">
-        <x:v>29</x:v>
+        <x:v>31</x:v>
       </x:c>
     </x:row>
     <x:row r="8">
       <x:c r="A8" s="4" t="s">
-        <x:v>30</x:v>
+        <x:v>32</x:v>
       </x:c>
       <x:c r="B8" s="4" t="s">
-        <x:v>31</x:v>
+        <x:v>33</x:v>
       </x:c>
       <x:c r="C8" s="4" t="s">
-        <x:v>7</x:v>
+        <x:v>29</x:v>
       </x:c>
       <x:c r="D8" s="4" t="s">
-        <x:v>32</x:v>
+        <x:v>34</x:v>
       </x:c>
       <x:c r="E8" s="4" t="s">
-        <x:v>33</x:v>
+        <x:v>35</x:v>
       </x:c>
     </x:row>
     <x:row r="9">
       <x:c r="A9" s="4" t="s">
-        <x:v>34</x:v>
+        <x:v>36</x:v>
       </x:c>
       <x:c r="B9" s="4" t="s">
-        <x:v>35</x:v>
+        <x:v>37</x:v>
       </x:c>
       <x:c r="C9" s="4" t="s">
-        <x:v>7</x:v>
+        <x:v>29</x:v>
       </x:c>
       <x:c r="D9" s="4" t="s">
-        <x:v>36</x:v>
+        <x:v>38</x:v>
       </x:c>
       <x:c r="E9" s="4" t="s">
-        <x:v>37</x:v>
+        <x:v>39</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>